<commit_message>
se crea nuevos cambios
</commit_message>
<xml_diff>
--- a/CREAR-OT-MAXIMO/datos excel/datos_OT.xlsx
+++ b/CREAR-OT-MAXIMO/datos excel/datos_OT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eruhern\Documents\UiPath\CREAR-OT-MAXIMO\datos excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F051E261-8764-45E9-997E-5D494165DE3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84096919-D73A-412F-83EE-B190104231BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="14980" activeTab="1" xr2:uid="{8B51D6BE-9F50-4663-859D-D701AB2BE83D}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>OT NUEVA</t>
   </si>
@@ -62,79 +62,31 @@
     <t>id</t>
   </si>
   <si>
-    <t>OT DICIEMBRE</t>
+    <t>MPI_CUATRIMESTRAL_03-20_PUERTO BERRIO</t>
   </si>
   <si>
-    <t>codigo</t>
+    <t>GD042</t>
   </si>
   <si>
-    <t>sitio</t>
+    <t>MPI_SEMESTRAL_03-20_SAN JOSE DEL NUS</t>
   </si>
   <si>
-    <t>REGION</t>
+    <t>GD234</t>
   </si>
   <si>
-    <t>CENTRO MTTO</t>
+    <t>MPI_SEMESTRAL_03-20_LA DANTA</t>
   </si>
   <si>
-    <t>RMC ASIGNADO WFM</t>
+    <t>GD352</t>
   </si>
   <si>
-    <t>S16886</t>
+    <t>S2230</t>
   </si>
   <si>
-    <t>YARUMAL</t>
+    <t>S8404</t>
   </si>
   <si>
-    <t>NOROCCIDENTE</t>
-  </si>
-  <si>
-    <t>TEM MEDELLIN</t>
-  </si>
-  <si>
-    <t>NORBEY ANDRES CARDONA FLOREZ</t>
-  </si>
-  <si>
-    <t>S9671</t>
-  </si>
-  <si>
-    <t>SANTA ROSA DE OSOS II</t>
-  </si>
-  <si>
-    <t>S5879</t>
-  </si>
-  <si>
-    <t>DON MATIAS DOS</t>
-  </si>
-  <si>
-    <t>S6085</t>
-  </si>
-  <si>
-    <t>YARUMAL II</t>
-  </si>
-  <si>
-    <t>MPI_TRIMESTRAL_01-20_YARUMAL</t>
-  </si>
-  <si>
-    <t>MPI_SEMESTRAL_01-20_DON MATIAS DOS</t>
-  </si>
-  <si>
-    <t>MPI_SEMESTRAL_01-20_YARUMAL II</t>
-  </si>
-  <si>
-    <t>MPI_SEMESTRAL_01-20_SANTA ROSA DE OSOS II</t>
-  </si>
-  <si>
-    <t>INF_S16886</t>
-  </si>
-  <si>
-    <t>GD091</t>
-  </si>
-  <si>
-    <t>GD018</t>
-  </si>
-  <si>
-    <t>UD405</t>
+    <t>S9796</t>
   </si>
 </sst>
 </file>
@@ -390,17 +342,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -718,10 +670,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BEBE62-703C-4EDF-9FCC-A1DE376903C0}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,7 +681,7 @@
     <col min="1" max="1" width="18.81640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="23" style="4" customWidth="1"/>
     <col min="3" max="3" width="38.6328125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.6328125" style="5" customWidth="1"/>
     <col min="5" max="5" width="14.08984375" customWidth="1"/>
     <col min="6" max="6" width="12.26953125" customWidth="1"/>
   </cols>
@@ -750,59 +702,51 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>43858.3125</v>
+        <v>43915</v>
       </c>
       <c r="B2" s="3">
-        <v>43858.75</v>
+        <v>43915</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
-        <v>43858.3125</v>
+        <v>43901</v>
       </c>
       <c r="B3" s="3">
-        <v>43858.75</v>
+        <v>43901</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
-        <v>43859.3125</v>
+        <v>43903</v>
       </c>
       <c r="B4" s="3">
-        <v>43859.75</v>
+        <v>43903</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>43860.3125</v>
-      </c>
-      <c r="B5" s="3">
-        <v>43860.75</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
@@ -1253,12 +1197,6 @@
       <c r="B80" s="3"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1270,100 +1208,335 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0DE604-C69A-41D3-BF4A-A25B2D89289E}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="18">
-        <v>5197232</v>
-      </c>
-      <c r="D2" s="18">
-        <v>5197234</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>25</v>
+      <c r="B2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="16">
+        <v>5297292</v>
+      </c>
+      <c r="D2" s="16">
+        <v>5297294</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="18">
-        <v>5197235</v>
-      </c>
-      <c r="D3" s="18">
-        <v>5197238</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>26</v>
+      <c r="A3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="16">
+        <v>5297298</v>
+      </c>
+      <c r="D3" s="16">
+        <v>5297300</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="18">
-        <v>5197239</v>
-      </c>
-      <c r="D4" s="18">
-        <v>5197240</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>27</v>
+      <c r="A4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="16">
+        <v>5297301</v>
+      </c>
+      <c r="D4" s="16">
+        <v>5297302</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="18">
-        <v>5197241</v>
-      </c>
-      <c r="D5" s="18">
-        <v>5197243</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>28</v>
-      </c>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1375,118 +1548,58 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>12</v>
-      </c>
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="11">
-        <v>5139785</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="11">
-        <v>5138568</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="11">
-        <v>5138585</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="11">
-        <v>5138855</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="16"/>
+      <c r="A6" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>